<commit_message>
super:change from superset to dashboards
</commit_message>
<xml_diff>
--- a/config/forms/app/super.xlsx
+++ b/config/forms/app/super.xlsx
@@ -45,13 +45,13 @@
     <t>str</t>
   </si>
   <si>
-    <t xml:space="preserve">Click the button below to go to superset </t>
+    <t>Click the button below to view the dashboards</t>
   </si>
   <si>
     <t>suoer</t>
   </si>
   <si>
-    <t>[&lt;span style='background-color: #648af7; color:white; padding: 1em; text-decoration: none;border-radius: 8px; '&gt;Superset&lt;/span&gt;](https://superset.openelis-global.org/superset/welcome/)</t>
+    <t>[&lt;span style='background-color: #648af7; color:white; padding: 1em; text-decoration: none;border-radius: 8px; '&gt;Dashboard&lt;/span&gt;](https://superset.openelis-global.org/superset/welcome/)</t>
   </si>
   <si>
     <t>end group</t>

</xml_diff>